<commit_message>
Created TC01 for ICDC MGT01 Study
</commit_message>
<xml_diff>
--- a/InputFiles/ICDC/TC01_ICDC_MGT01_Breed-LabradorRetriever.xlsx
+++ b/InputFiles/ICDC/TC01_ICDC_MGT01_Breed-LabradorRetriever.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohilz2/Automation/poc-07-15-2024/Commons_Automation/InputFiles/ICDC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D3C3A9F-12DA-8B42-A279-EBF79735BD44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0314CA7D-7B19-FA45-B202-0D13C7472F2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32760" yWindow="-880" windowWidth="42480" windowHeight="27840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -89,51 +89,6 @@
     st.clinical_study_designation = 'MGT01' AND dmg.breed = 'Labrador Retriever';</t>
   </si>
   <si>
-    <t>SELECT
-    DISTINCT c.case_id AS "Case ID",
-    st.clinical_study_designation AS "Study Code",
-    st.clinical_study_type AS "Study Type",
-    dmg.breed AS "Breed",
-    diag.disease_term AS "Diagnosis",
-    diag.stage_of_disease AS "Stage Of Disease",
-    COALESCE(CAST(dmg.patient_age_at_enrollment AS INT), '') AS "Age", 
-    COALESCE(TRIM(dmg.sex), '') AS "Sex",   
-    COALESCE(dmg.neutered_indicator, '') AS "Neutered Status",  
-    COALESCE(
-        CASE 
-            WHEN dmg.weight = CAST(dmg.weight AS INT) THEN CAST(dmg.weight AS INT)
-            ELSE dmg.weight 
-        END, 
-    '') AS "Weight (kg)",        
-    COALESCE(diag.best_response, '') AS "Response to Treatment",  
-    COALESCE("", '') AS "Cohort"  
-FROM 
-    df_case c
-JOIN 
-    df_study st ON c."study.clinical_study_designation" = st.clinical_study_designation
-JOIN 
-    df_demographic dmg ON dmg."case.case_id" = c.case_id
-JOIN 
-    df_diagnosis diag ON diag."case.case_id" = c.case_id
-JOIN 
-    df_enrollment enr ON enr."case.case_id" = c.case_id
-JOIN 
-    df_program p ON st."program.program_acronym" = p.program_acronym
-JOIN 
-    df_sample smp ON smp."case.case_id" = c.case_id
-JOIN 
-    df_publication pub ON pub."study.clinical_study_designation" = st.clinical_study_designation
-LEFT JOIN 
-    df_case_file cf ON cf."sample.sample_id" = smp.sample_id
-LEFT JOIN 
-    df_study_file sf ON sf."study.clinical_study_designation" = st.clinical_study_designation
-WHERE
-    st.clinical_study_designation = 'MGT01' AND dmg.breed = 'Labrador Retriever'
-ORDER BY 
-    c.case_id ASC
-LIMIT 100;</t>
-  </si>
-  <si>
     <t>SELECT DISTINCT
     smp.sample_id AS "Sample ID",
     c.case_id AS "Case ID",
@@ -171,67 +126,6 @@
    st.clinical_study_designation = 'MGT01' AND dmg.breed = 'Labrador Retriever'
 ORDER BY 
     smp.sample_id ASC
-LIMIT 100;</t>
-  </si>
-  <si>
-    <t>SELECT DISTINCT
-    cf.file_name AS "File Name",
-    CASE
-        WHEN cf.file_name LIKE '%.bai' THEN 'bai'
-        WHEN cf.file_name LIKE '%.bam' THEN 'bam'
-        WHEN cf.file_name LIKE '%.csv' THEN 'csv'
-        WHEN cf.file_name LIKE '%.doc' THEN 'doc'
-        WHEN cf.file_name LIKE '%.docx' THEN 'docx'
-        WHEN cf.file_name LIKE '%.gz' THEN 'gz'
-        WHEN cf.file_name LIKE '%.pdf' THEN 'pdf'
-        WHEN cf.file_name LIKE '%.rtf' THEN 'rtf'
-        WHEN cf.file_name LIKE '%.tbi' THEN 'tbi'
-        WHEN cf.file_name LIKE '%.tif' THEN 'tif'
-        WHEN cf.file_name LIKE '%.xls' THEN 'xls'
-        WHEN cf.file_name LIKE '%.xlsx' THEN 'xlsx'
-        ELSE 'Unknown'
-    END AS "Format",
-    cf.file_type AS "File Type",
-    CASE     
-    WHEN cf.original_file_size &gt;= 1024 * 1024 * 1024 THEN 
-        ROUND(cf.original_file_size / (1024.0 * 1024.0 * 1024.0), 2) || ' GB' 
-    WHEN cf.original_file_size &gt;= 1024 * 1024 THEN 
-        ROUND(cf.original_file_size / (1024.0 * 1024.0), 2) || ' MB' 
-    WHEN cf.original_file_size &gt;= 1024 THEN 
-        ROUND(cf.original_file_size / 1024.0, 2) || ' KB' 
-    ELSE 
-        ROUND(cf.original_file_size, 2) || ' Bytes' 
-END AS "Size",
-    'sample' AS "Association",
-    cf.file_description AS "Description",
-    smp.sample_id AS "Sample ID",
-    c.case_id AS "Case ID",
-    dmg.breed AS "Breed",
-    diag.disease_term AS "Diagnosis"
-FROM 
-    df_case_file cf
-JOIN 
-    df_sample smp ON cf."sample.sample_id" = smp.sample_id
-JOIN 
-    df_case c ON smp."case.case_id" = c.case_id
-JOIN 
-    df_study st ON c."study.clinical_study_designation" = st.clinical_study_designation
-JOIN 
-    df_program p ON st."program.program_acronym" = p.program_acronym
-JOIN 
-    df_demographic dmg ON dmg."case.case_id" = c.case_id
-JOIN 
-    df_diagnosis diag ON diag."case.case_id" = c.case_id
-JOIN 
-    df_enrollment enr ON enr."case.case_id" = c.case_id
-JOIN 
-    df_publication pub ON pub."study.clinical_study_designation" = st.clinical_study_designation
-LEFT JOIN 
-    df_study_file sf ON sf."study.clinical_study_designation" = st.clinical_study_designation
-WHERE
-    st.clinical_study_designation = 'MGT01' AND dmg.breed = 'Labrador Retriever'
-ORDER BY 
-    sf.file_name ASC
 LIMIT 100;</t>
   </si>
   <si>
@@ -298,14 +192,136 @@
   <si>
     <t>TC01_ICDC_MGT01_Breed-LabradorRetriever_WebData.xlsx</t>
   </si>
+  <si>
+    <t>SELECT
+    DISTINCT c.case_id AS "Case ID",
+    st.clinical_study_designation AS "Study Code",
+    st.clinical_study_type AS "Study Type",
+    dmg.breed AS "Breed",
+    diag.disease_term AS "Diagnosis",
+    diag.stage_of_disease AS "Stage Of Disease",
+    dmg.patient_age_at_enrollment AS "Age", 
+    COALESCE(TRIM(dmg.sex), '') AS "Sex",   
+    COALESCE(dmg.neutered_indicator, '') AS "Neutered Status",  
+    COALESCE(
+        CASE 
+            WHEN dmg.weight = CAST(dmg.weight AS INT) THEN CAST(dmg.weight AS INT)
+            ELSE dmg.weight 
+        END, 
+    '') AS "Weight (kg)",        
+    COALESCE(diag.best_response, '') AS "Response to Treatment",  
+    COALESCE(coh.cohort_description, '') AS "Cohort"  
+FROM 
+    df_case c
+JOIN 
+    df_study st ON c."study.clinical_study_designation" = st.clinical_study_designation
+JOIN 
+    df_demographic dmg ON dmg."case.case_id" = c.case_id
+JOIN 
+    df_diagnosis diag ON diag."case.case_id" = c.case_id
+JOIN 
+    df_enrollment enr ON enr."case.case_id" = c.case_id
+JOIN 
+    df_program p ON st."program.program_acronym" = p.program_acronym
+JOIN 
+    df_sample smp ON smp."case.case_id" = c.case_id
+JOIN 
+    df_publication pub ON pub."study.clinical_study_designation" = st.clinical_study_designation
+LEFT JOIN 
+    df_case_file cf ON cf."sample.sample_id" = smp.sample_id
+LEFT JOIN 
+    df_study_file sf ON sf."study.clinical_study_designation" = st.clinical_study_designation
+LEFT JOIN
+    df_cohort coh ON coh."study.clinical_study_designation" = st.clinical_study_designation
+WHERE
+     st.clinical_study_designation = 'MGT01' AND dmg.breed = 'Labrador Retriever'
+ORDER BY 
+    c.case_id ASC
+LIMIT 100;</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT
+    cf.file_name AS "File Name",
+    CASE
+        WHEN cf.file_name LIKE '%.bai' THEN 'bai'
+        WHEN cf.file_name LIKE '%.bam' THEN 'bam'
+        WHEN cf.file_name LIKE '%.csv' THEN 'csv'
+        WHEN cf.file_name LIKE '%.doc' THEN 'doc'
+        WHEN cf.file_name LIKE '%.docx' THEN 'docx'
+        WHEN cf.file_name LIKE '%.gz' THEN 'gz'
+        WHEN cf.file_name LIKE '%.pdf' THEN 'pdf'
+        WHEN cf.file_name LIKE '%.rtf' THEN 'rtf'
+        WHEN cf.file_name LIKE '%.tbi' THEN 'tbi'
+        WHEN cf.file_name LIKE '%.tif' THEN 'tif'
+        WHEN cf.file_name LIKE '%.xls' THEN 'xls'
+        WHEN cf.file_name LIKE '%.xlsx' THEN 'xlsx'
+        ELSE 'Unknown'
+    END AS "Format",
+    cf.file_type AS "File Type",
+    CASE     
+    WHEN cf.file_size &gt;= 1024 * 1024 * 1024 THEN 
+        ROUND(cf.file_size / (1024.0 * 1024.0 * 1024.0), 2) || ' GB' 
+    WHEN cf.file_size &gt;= 1024 * 1024 THEN 
+        ROUND(cf.file_size / (1024.0 * 1024.0), 2) || ' MB' 
+    WHEN cf.file_size &gt;= 1024 THEN 
+        ROUND(cf.file_size / 1024.0, 2) || ' KB' 
+    ELSE 
+        ROUND(cf.file_size, 2) || ' Bytes' 
+END AS "Size",
+    'sample' AS "Association",
+    cf.file_description AS "Description",
+    smp.sample_id AS "Sample ID",
+    c.case_id AS "Case ID",
+    dmg.breed AS "Breed",
+    diag.disease_term AS "Diagnosis"
+FROM 
+    df_case_file cf
+JOIN 
+    df_sample smp ON cf."sample.sample_id" = smp.sample_id
+JOIN 
+    df_case c ON smp."case.case_id" = c.case_id
+JOIN 
+    df_study st ON c."study.clinical_study_designation" = st.clinical_study_designation
+JOIN 
+    df_program p ON st."program.program_acronym" = p.program_acronym
+JOIN 
+    df_demographic dmg ON dmg."case.case_id" = c.case_id
+JOIN 
+    df_diagnosis diag ON diag."case.case_id" = c.case_id
+JOIN 
+    df_enrollment enr ON enr."case.case_id" = c.case_id
+JOIN 
+    df_publication pub ON pub."study.clinical_study_designation" = st.clinical_study_designation
+LEFT JOIN 
+    df_study_file sf ON sf."study.clinical_study_designation" = st.clinical_study_designation
+WHERE
+    st.clinical_study_designation = 'MGT01' AND dmg.breed = 'Labrador Retriever'
+ORDER BY 
+    sf.file_name ASC
+LIMIT 100;</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -358,11 +374,17 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -688,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -721,17 +743,17 @@
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
@@ -739,7 +761,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -747,8 +769,8 @@
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>12</v>
+      <c r="B4" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -757,7 +779,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1"/>
     </row>
@@ -765,7 +787,7 @@
       <c r="C6" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated ICDC queries and ICDC Utils.py
</commit_message>
<xml_diff>
--- a/InputFiles/ICDC/TC01_ICDC_MGT01_Breed-LabradorRetriever.xlsx
+++ b/InputFiles/ICDC/TC01_ICDC_MGT01_Breed-LabradorRetriever.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sohilz2/Automation/poc-07-15-2024/Commons_Automation/InputFiles/ICDC/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0314CA7D-7B19-FA45-B202-0D13C7472F2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB308FE5-69BD-0740-BEDF-7CE18C046E19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32760" yWindow="-880" windowWidth="42480" windowHeight="27840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -60,10 +60,93 @@
     <t>CaseFilesTab</t>
   </si>
   <si>
+    <t>TC01_ICDC_MGT01_Breed-LabradorRetriever_TSVData.xlsx</t>
+  </si>
+  <si>
+    <t>TC01_ICDC_MGT01_Breed-LabradorRetriever_WebData.xlsx</t>
+  </si>
+  <si>
+    <t>SELECT 
+    DISTINCT cf.file_name AS "File Name",
+    CASE
+        WHEN cf.file_name LIKE '%.bai' THEN 'bai'
+        WHEN cf.file_name LIKE '%.bam' THEN 'bam'
+        WHEN cf.file_name LIKE '%.csv' THEN 'csv'
+        WHEN cf.file_name LIKE '%.doc' THEN 'doc'
+        WHEN cf.file_name LIKE '%.docx' THEN 'docx'
+        WHEN cf.file_name LIKE '%.gz' THEN 'gz'
+        WHEN cf.file_name LIKE '%.pdf' THEN 'pdf'
+        WHEN cf.file_name LIKE '%.rtf' THEN 'rtf'
+        WHEN cf.file_name LIKE '%.tbi' THEN 'tbi'
+        WHEN cf.file_name LIKE '%.tif' THEN 'tif'
+        WHEN cf.file_name LIKE '%.xls' THEN 'xls'
+        WHEN cf.file_name LIKE '%.xlsx' THEN 'xlsx'
+        ELSE 'Unknown'
+    END AS "Format",
+    cf.file_type AS "File Type",
+    CASE     
+    WHEN cf.file_size &gt;= 1024 * 1024 * 1024 THEN 
+        CASE 
+            WHEN ROUND(cf.file_size / (1024.0 * 1024.0 * 1024.0), 2) = CAST(ROUND(cf.file_size / (1024.0 * 1024.0 * 1024.0), 0) AS INT) 
+            THEN CAST(CAST(ROUND(cf.file_size / (1024.0 * 1024.0 * 1024.0), 0) AS INT) AS TEXT) || ' GB'
+            ELSE ROUND(cf.file_size / (1024.0 * 1024.0 * 1024.0), 2) || ' GB'
+        END
+    WHEN cf.file_size &gt;= 1024 * 1024 THEN 
+        CASE 
+            WHEN ROUND(cf.file_size / (1024.0 * 1024.0), 2) = CAST(ROUND(cf.file_size / (1024.0 * 1024.0), 0) AS INT) 
+            THEN CAST(CAST(ROUND(cf.file_size / (1024.0 * 1024.0), 0) AS INT) AS TEXT) || ' MB'
+            ELSE ROUND(cf.file_size / (1024.0 * 1024.0), 2) || ' MB'
+        END
+    WHEN cf.file_size &gt;= 1024 THEN 
+        CASE 
+            WHEN ROUND(cf.file_size / 1024.0, 2) = CAST(ROUND(cf.file_size / 1024.0, 0) AS INT) 
+            THEN CAST(CAST(ROUND(cf.file_size / 1024.0, 0) AS INT) AS TEXT) || ' KB'
+            ELSE ROUND(cf.file_size / 1024.0, 2) || ' KB'
+        END
+    ELSE 
+        CASE 
+            WHEN ROUND(cf.file_size, 2) = CAST(ROUND(cf.file_size, 0) AS INT) 
+            THEN CAST(CAST(ROUND(cf.file_size, 0) AS INT) AS TEXT) || ' Bytes'
+            ELSE ROUND(cf.file_size, 2) || ' Bytes'
+        END
+END AS "Size",
+    'sample' AS "Association",
+    cf.file_description AS "Description",
+    smp.sample_id AS "Sample ID",
+    c.case_record_id AS "Case ID",
+    dmg.breed AS "Breed",
+    diag.disease_term AS "Diagnosis"
+FROM 
+    df_case_file cf
+JOIN 
+    df_sample smp ON cf."sample.sample_id" = smp.sample_id
+JOIN 
+    df_case c ON smp."case.case_record_id" = c.case_record_id
+JOIN 
+    df_study st ON c."study.clinical_study_designation" = st.clinical_study_designation
+JOIN 
+    df_program p ON st."program.program_acronym" = p.program_acronym
+JOIN 
+    df_demographic dmg ON dmg."case.case_record_id" = c.case_record_id
+JOIN 
+    df_diagnosis diag ON diag."case.case_record_id" = c.case_record_id
+JOIN 
+    df_enrollment enr ON enr."case.case_record_id" = c.case_record_id
+JOIN 
+    df_publication pub ON pub."study.clinical_study_designation" = st.clinical_study_designation
+LEFT JOIN 
+    df_study_file sf ON sf."study.clinical_study_designation" = st.clinical_study_designation
+WHERE
+    st.clinical_study_designation = 'MGT01' AND dmg.breed = 'Labrador Retriever'
+ORDER BY 
+    cf.file_name ASC
+LIMIT 100;</t>
+  </si>
+  <si>
     <t>SELECT
     COUNT(DISTINCT p.program_acronym) AS "Programs",
     COUNT(DISTINCT st.clinical_study_designation) AS "Studies",
-    COUNT(DISTINCT c.case_id) AS "Cases",
+    COUNT(DISTINCT c.case_record_id) AS "Cases",
     COUNT(DISTINCT smp.sample_id) AS "Samples",
     COUNT(DISTINCT cf.file_name) AS "Case Files",         
     COUNT(DISTINCT sf.file_name) AS "Study Files" 
@@ -74,13 +157,13 @@
 JOIN 
     df_case c ON st.clinical_study_designation = c."study.clinical_study_designation"
 JOIN 
-    df_demographic dmg ON dmg."case.case_id" = c.case_id
-JOIN 
-    df_diagnosis diag ON diag."case.case_id" = c.case_id
-JOIN 
-    df_enrollment enr ON enr."case.case_id" = c.case_id
-JOIN 
-    df_sample smp ON smp."case.case_id" = c.case_id
+    df_demographic dmg ON dmg."case.case_record_id" = c.case_record_id
+JOIN 
+    df_diagnosis diag ON diag."case.case_record_id" = c.case_record_id
+JOIN 
+    df_enrollment enr ON enr."case.case_record_id" = c.case_record_id
+JOIN 
+    df_sample smp ON smp."case.case_record_id" = c.case_record_id
 LEFT JOIN 
     df_case_file cf ON cf."sample.sample_id" = smp.sample_id
 LEFT JOIN 
@@ -89,9 +172,60 @@
     st.clinical_study_designation = 'MGT01' AND dmg.breed = 'Labrador Retriever';</t>
   </si>
   <si>
+    <t>SELECT
+    DISTINCT c.case_record_id AS "Case ID",
+    st.clinical_study_designation AS "Study Code",
+    st.clinical_study_type AS "Study Type",
+    dmg.breed AS "Breed",
+    diag.disease_term AS "Diagnosis",
+    diag.stage_of_disease AS "Stage Of Disease",
+    CASE 
+    WHEN dmg.patient_age_at_enrollment = CAST(dmg.patient_age_at_enrollment AS INT) 
+    THEN CAST(CAST(dmg.patient_age_at_enrollment AS INT) AS TEXT)
+    ELSE CAST(dmg.patient_age_at_enrollment AS TEXT)
+END AS "Age", 
+    COALESCE(TRIM(dmg.sex), '') AS "Sex",   
+    COALESCE(dmg.neutered_indicator, '') AS "Neutered Status",  
+    COALESCE(
+        CASE 
+            WHEN dmg.weight = CAST(dmg.weight AS INT) THEN CAST(dmg.weight AS INT)
+            ELSE dmg.weight 
+        END, 
+    '') AS "Weight (kg)",        
+    COALESCE(diag.best_response, '') AS "Response to Treatment",  
+    COALESCE(coh.cohort_description, '') AS "Cohort"  
+FROM 
+    df_case c
+JOIN 
+    df_study st ON c."study.clinical_study_designation" = st.clinical_study_designation
+JOIN 
+    df_demographic dmg ON dmg."case.case_record_id" = c.case_record_id
+JOIN 
+    df_diagnosis diag ON diag."case.case_record_id" = c.case_record_id
+JOIN 
+    df_enrollment enr ON enr."case.case_record_id" = c.case_record_id
+JOIN 
+    df_program p ON st."program.program_acronym" = p.program_acronym
+JOIN 
+    df_sample smp ON smp."case.case_record_id" = c.case_record_id
+JOIN 
+    df_publication pub ON pub."study.clinical_study_designation" = st.clinical_study_designation
+LEFT JOIN 
+    df_case_file cf ON cf."sample.sample_id" = smp.sample_id
+LEFT JOIN 
+    df_study_file sf ON sf."study.clinical_study_designation" = st.clinical_study_designation
+LEFT JOIN
+    df_cohort coh ON coh."study.clinical_study_designation" = st.clinical_study_designation
+WHERE
+    st.clinical_study_designation = 'MGT01' AND dmg.breed = 'Labrador Retriever'
+ORDER BY 
+    c.case_record_id ASC
+LIMIT 100;</t>
+  </si>
+  <si>
     <t>SELECT DISTINCT
     smp.sample_id AS "Sample ID",
-    c.case_id AS "Case ID",
+    c.case_record_id AS "Case ID",
     COALESCE(dmg.breed, '') AS "Breed",
     COALESCE(diag.disease_term, '') AS "Diagnosis",
     COALESCE(smp.sample_site, '') AS "Sample Site",
@@ -105,15 +239,15 @@
 FROM 
     df_sample smp
 JOIN 
-    df_case c ON smp."case.case_id" = c.case_id
+    df_case c ON smp."case.case_record_id" = c.case_record_id
 JOIN 
     df_publication pub ON pub."study.clinical_study_designation" = st.clinical_study_designation
 JOIN 
-    df_demographic dmg ON dmg."case.case_id" = c.case_id
-JOIN 
-    df_diagnosis diag ON diag."case.case_id" = c.case_id
-JOIN 
-    df_enrollment enr ON enr."case.case_id" = c.case_id
+    df_demographic dmg ON dmg."case.case_record_id" = c.case_record_id
+JOIN 
+    df_diagnosis diag ON diag."case.case_record_id" = c.case_record_id
+JOIN 
+    df_enrollment enr ON enr."case.case_record_id" = c.case_record_id
 JOIN 
     df_program p ON st."program.program_acronym" = p.program_acronym
 JOIN 
@@ -150,14 +284,14 @@
         ELSE 'Unknown'
     END AS "Format",
     CASE     
-        WHEN sf.original_file_size &gt;= 1024 * 1024 * 1024 THEN 
-            ROUND(sf.original_file_size / (1024.0 * 1024.0 * 1024.0), 2) || ' GB' 
-        WHEN sf.original_file_size &gt;= 1024 * 1024 THEN 
-            ROUND(sf.original_file_size / (1024.0 * 1024.0), 2) || ' MB' 
-        WHEN sf.original_file_size &gt;= 1024 THEN 
-            ROUND(sf.original_file_size / 1024.0, 2) || ' KB' 
+        WHEN sf.file_size &gt;= 1024 * 1024 * 1024 THEN 
+            ROUND(sf.file_size / (1024.0 * 1024.0 * 1024.0), 2) || ' GB' 
+        WHEN sf.file_size &gt;= 1024 * 1024 THEN 
+            ROUND(sf.file_size / (1024.0 * 1024.0), 2) || ' MB' 
+        WHEN sf.file_size &gt;= 1024 THEN 
+            ROUND(sf.file_size / 1024.0, 2) || ' KB' 
         ELSE 
-            ROUND(sf.original_file_size, 2) || ' Bytes' 
+            ROUND(sf.file_size, 2) || ' Bytes' 
     END AS "Size",
     st.clinical_study_designation AS "Study Code"
 FROM 
@@ -165,17 +299,17 @@
 JOIN 
     df_sample smp ON cf."sample.sample_id" = smp.sample_id
 JOIN 
-    df_case c ON smp."case.case_id" = c.case_id
+    df_case c ON smp."case.case_record_id" = c.case_record_id
 JOIN 
     df_study st ON c."study.clinical_study_designation" = st.clinical_study_designation
 JOIN 
     df_program p ON st."program.program_acronym" = p.program_acronym
 JOIN 
-    df_demographic dmg ON dmg."case.case_id" = c.case_id
-JOIN 
-    df_diagnosis diag ON diag."case.case_id" = c.case_id
-JOIN 
-    df_enrollment enr ON enr."case.case_id" = c.case_id
+    df_demographic dmg ON dmg."case.case_record_id" = c.case_record_id
+JOIN 
+    df_diagnosis diag ON diag."case.case_record_id" = c.case_record_id
+JOIN 
+    df_enrollment enr ON enr."case.case_record_id" = c.case_record_id
 JOIN 
     df_publication pub ON pub."study.clinical_study_designation" = st.clinical_study_designation
 LEFT JOIN 
@@ -186,135 +320,14 @@
     sf.file_name ASC
 LIMIT 100;</t>
   </si>
-  <si>
-    <t>TC01_ICDC_MGT01_Breed-LabradorRetriever_TSVData.xlsx</t>
-  </si>
-  <si>
-    <t>TC01_ICDC_MGT01_Breed-LabradorRetriever_WebData.xlsx</t>
-  </si>
-  <si>
-    <t>SELECT
-    DISTINCT c.case_id AS "Case ID",
-    st.clinical_study_designation AS "Study Code",
-    st.clinical_study_type AS "Study Type",
-    dmg.breed AS "Breed",
-    diag.disease_term AS "Diagnosis",
-    diag.stage_of_disease AS "Stage Of Disease",
-    dmg.patient_age_at_enrollment AS "Age", 
-    COALESCE(TRIM(dmg.sex), '') AS "Sex",   
-    COALESCE(dmg.neutered_indicator, '') AS "Neutered Status",  
-    COALESCE(
-        CASE 
-            WHEN dmg.weight = CAST(dmg.weight AS INT) THEN CAST(dmg.weight AS INT)
-            ELSE dmg.weight 
-        END, 
-    '') AS "Weight (kg)",        
-    COALESCE(diag.best_response, '') AS "Response to Treatment",  
-    COALESCE(coh.cohort_description, '') AS "Cohort"  
-FROM 
-    df_case c
-JOIN 
-    df_study st ON c."study.clinical_study_designation" = st.clinical_study_designation
-JOIN 
-    df_demographic dmg ON dmg."case.case_id" = c.case_id
-JOIN 
-    df_diagnosis diag ON diag."case.case_id" = c.case_id
-JOIN 
-    df_enrollment enr ON enr."case.case_id" = c.case_id
-JOIN 
-    df_program p ON st."program.program_acronym" = p.program_acronym
-JOIN 
-    df_sample smp ON smp."case.case_id" = c.case_id
-JOIN 
-    df_publication pub ON pub."study.clinical_study_designation" = st.clinical_study_designation
-LEFT JOIN 
-    df_case_file cf ON cf."sample.sample_id" = smp.sample_id
-LEFT JOIN 
-    df_study_file sf ON sf."study.clinical_study_designation" = st.clinical_study_designation
-LEFT JOIN
-    df_cohort coh ON coh."study.clinical_study_designation" = st.clinical_study_designation
-WHERE
-     st.clinical_study_designation = 'MGT01' AND dmg.breed = 'Labrador Retriever'
-ORDER BY 
-    c.case_id ASC
-LIMIT 100;</t>
-  </si>
-  <si>
-    <t>SELECT DISTINCT
-    cf.file_name AS "File Name",
-    CASE
-        WHEN cf.file_name LIKE '%.bai' THEN 'bai'
-        WHEN cf.file_name LIKE '%.bam' THEN 'bam'
-        WHEN cf.file_name LIKE '%.csv' THEN 'csv'
-        WHEN cf.file_name LIKE '%.doc' THEN 'doc'
-        WHEN cf.file_name LIKE '%.docx' THEN 'docx'
-        WHEN cf.file_name LIKE '%.gz' THEN 'gz'
-        WHEN cf.file_name LIKE '%.pdf' THEN 'pdf'
-        WHEN cf.file_name LIKE '%.rtf' THEN 'rtf'
-        WHEN cf.file_name LIKE '%.tbi' THEN 'tbi'
-        WHEN cf.file_name LIKE '%.tif' THEN 'tif'
-        WHEN cf.file_name LIKE '%.xls' THEN 'xls'
-        WHEN cf.file_name LIKE '%.xlsx' THEN 'xlsx'
-        ELSE 'Unknown'
-    END AS "Format",
-    cf.file_type AS "File Type",
-    CASE     
-    WHEN cf.file_size &gt;= 1024 * 1024 * 1024 THEN 
-        ROUND(cf.file_size / (1024.0 * 1024.0 * 1024.0), 2) || ' GB' 
-    WHEN cf.file_size &gt;= 1024 * 1024 THEN 
-        ROUND(cf.file_size / (1024.0 * 1024.0), 2) || ' MB' 
-    WHEN cf.file_size &gt;= 1024 THEN 
-        ROUND(cf.file_size / 1024.0, 2) || ' KB' 
-    ELSE 
-        ROUND(cf.file_size, 2) || ' Bytes' 
-END AS "Size",
-    'sample' AS "Association",
-    cf.file_description AS "Description",
-    smp.sample_id AS "Sample ID",
-    c.case_id AS "Case ID",
-    dmg.breed AS "Breed",
-    diag.disease_term AS "Diagnosis"
-FROM 
-    df_case_file cf
-JOIN 
-    df_sample smp ON cf."sample.sample_id" = smp.sample_id
-JOIN 
-    df_case c ON smp."case.case_id" = c.case_id
-JOIN 
-    df_study st ON c."study.clinical_study_designation" = st.clinical_study_designation
-JOIN 
-    df_program p ON st."program.program_acronym" = p.program_acronym
-JOIN 
-    df_demographic dmg ON dmg."case.case_id" = c.case_id
-JOIN 
-    df_diagnosis diag ON diag."case.case_id" = c.case_id
-JOIN 
-    df_enrollment enr ON enr."case.case_id" = c.case_id
-JOIN 
-    df_publication pub ON pub."study.clinical_study_designation" = st.clinical_study_designation
-LEFT JOIN 
-    df_study_file sf ON sf."study.clinical_study_designation" = st.clinical_study_designation
-WHERE
-    st.clinical_study_designation = 'MGT01' AND dmg.breed = 'Labrador Retriever'
-ORDER BY 
-    sf.file_name ASC
-LIMIT 100;</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -374,14 +387,11 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -710,8 +720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -743,25 +753,25 @@
       <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>10</v>
+      <c r="B3" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -769,8 +779,8 @@
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>15</v>
+      <c r="B4" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="C4" s="2"/>
     </row>
@@ -779,7 +789,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1"/>
     </row>
@@ -787,7 +797,7 @@
       <c r="C6" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>